<commit_message>
converting to osd256 commencted out old osd functions
</commit_message>
<xml_diff>
--- a/tools/16x20char_designer.xlsx
+++ b/tools/16x20char_designer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\00GIT\OSDeluxe\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE768F9B-6A6E-49B9-BB9C-9A23EC0DFB1A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B0C0D9-B644-4D28-ABE1-C929C83846E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="9120" xr2:uid="{7204D92D-006B-4887-9E42-7235DD687936}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="3">
   <si>
     <t>x</t>
   </si>
@@ -418,12 +418,13 @@
   <dimension ref="A1:BD44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25:U44"/>
+      <selection activeCell="W2" sqref="W2:W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16" width="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="43" customWidth="1"/>
     <col min="25" max="25" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="32" width="2" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="2.140625" bestFit="1" customWidth="1"/>
@@ -514,6 +515,10 @@
       <c r="U2">
         <f>IF(M2="o",64,0)+IF(M2="x",192,0)+IF(N2="o",16,0)+IF(N2="x",48,0)+IF(O2="o",4,0)+IF(O2="x",12,0)+IF(P2="o",1,0)+IF(P2="x",3,0)</f>
         <v>0</v>
+      </c>
+      <c r="W2" t="str">
+        <f>_xlfn.CONCAT(R2,",",S2,",",T2,",",U2,",")</f>
+        <v>0,0,0,0,</v>
       </c>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
@@ -584,6 +589,10 @@
         <f t="shared" ref="U3:U20" si="3">IF(M3="o",64,0)+IF(M3="x",192,0)+IF(N3="o",16,0)+IF(N3="x",48,0)+IF(O3="o",4,0)+IF(O3="x",12,0)+IF(P3="o",1,0)+IF(P3="x",3,0)</f>
         <v>0</v>
       </c>
+      <c r="W3" t="str">
+        <f t="shared" ref="W3:W44" si="4">_xlfn.CONCAT(R3,",",S3,",",T3,",",U3,",")</f>
+        <v>0,0,0,0,</v>
+      </c>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
@@ -620,31 +629,23 @@
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -653,56 +654,48 @@
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" si="4"/>
+        <v>0,0,80,64,</v>
       </c>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
-      <c r="AA4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK4" s="2"/>
+      <c r="AG4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
-      <c r="AO4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
       <c r="AS4" s="1"/>
@@ -720,113 +713,91 @@
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="J5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="P5" s="2"/>
       <c r="Q5" t="s">
         <v>1</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <f t="shared" si="1"/>
-        <v>253</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>245</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>208</v>
+      </c>
+      <c r="W5" t="str">
+        <f t="shared" si="4"/>
+        <v>0,1,245,208,</v>
       </c>
       <c r="Y5" s="2"/>
-      <c r="Z5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
       <c r="AF5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AG5" s="2"/>
+      <c r="AG5" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AH5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ5" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL5" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AM5" s="2"/>
-      <c r="AN5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
       <c r="AS5" s="1"/>
       <c r="AT5" s="1"/>
@@ -843,28 +814,20 @@
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="J6" s="2" t="s">
         <v>2</v>
       </c>
@@ -872,58 +835,54 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N6" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="P6" s="2"/>
       <c r="Q6" t="s">
         <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
-        <v>253</v>
+        <v>7</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>208</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="4"/>
+        <v>0,7,93,208,</v>
       </c>
       <c r="Y6" s="2"/>
-      <c r="Z6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
       <c r="AE6" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG6" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AH6" s="2" t="s">
         <v>2</v>
       </c>
@@ -931,25 +890,19 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL6" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AM6" s="2"/>
-      <c r="AN6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
       <c r="AR6" s="1"/>
       <c r="AS6" s="1"/>
       <c r="AT6" s="1"/>
@@ -965,26 +918,14 @@
       <c r="BD6" s="1"/>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>0</v>
@@ -999,52 +940,44 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="P7" s="2"/>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>65</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="4"/>
+        <v>0,7,93,208,</v>
+      </c>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
       <c r="AE7" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF7" s="2" t="s">
         <v>0</v>
@@ -1059,39 +992,27 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL7" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AM7" s="2"/>
-      <c r="AN7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
       <c r="AR7" s="1"/>
       <c r="AS7" s="1"/>
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
       <c r="AV7" s="1"/>
-      <c r="AW7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY7" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
+      <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
@@ -1099,24 +1020,14 @@
       <c r="BD7" s="1"/>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>0</v>
@@ -1131,50 +1042,44 @@
         <v>0</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="P8" s="2"/>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>65</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="4"/>
+        <v>0,7,93,208,</v>
+      </c>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AD8" s="2"/>
       <c r="AE8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>0</v>
@@ -1189,68 +1094,46 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL8" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AM8" s="2"/>
-      <c r="AN8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
       <c r="AR8" s="1"/>
       <c r="AS8" s="1"/>
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
-      <c r="AV8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
       <c r="BA8" s="1"/>
       <c r="BB8" s="1"/>
       <c r="BC8" s="1"/>
       <c r="BD8" s="1"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>0</v>
@@ -1265,50 +1148,48 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="O9" s="2"/>
-      <c r="P9" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="P9" s="2"/>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="T9">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>65</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="4"/>
+        <v>4,71,93,208,</v>
+      </c>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
       <c r="AA9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="2"/>
       <c r="AE9" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF9" s="2" t="s">
         <v>0</v>
@@ -1323,55 +1204,37 @@
         <v>0</v>
       </c>
       <c r="AJ9" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL9" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL9" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AM9" s="2"/>
-      <c r="AN9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
       <c r="AR9" s="1"/>
       <c r="AS9" s="1"/>
       <c r="AT9" s="1"/>
       <c r="AU9" s="1"/>
-      <c r="AV9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ9" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
       <c r="BA9" s="1"/>
       <c r="BB9" s="1"/>
       <c r="BC9" s="1"/>
       <c r="BD9" s="1"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
@@ -1380,60 +1243,62 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N10" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="O10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="P10" s="2"/>
       <c r="R10">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>29</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>215</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>253</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>69</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="4"/>
+        <v>29,215,253,244,</v>
+      </c>
+      <c r="Y10" s="2"/>
       <c r="Z10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA10" s="2" t="s">
         <v>0</v>
@@ -1442,69 +1307,51 @@
         <v>2</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AJ10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL10" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL10" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AM10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AN10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AR10" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
       <c r="AS10" s="1"/>
       <c r="AT10" s="1"/>
       <c r="AU10" s="1"/>
-      <c r="AV10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ10" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
       <c r="BA10" s="1"/>
       <c r="BB10" s="1"/>
       <c r="BC10" s="1"/>
@@ -1518,37 +1365,37 @@
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>2</v>
@@ -1557,23 +1404,27 @@
         <v>0</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R11">
         <f t="shared" si="0"/>
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>119</v>
       </c>
       <c r="T11">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>253</v>
       </c>
       <c r="U11">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>221</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="4"/>
+        <v>119,119,253,221,</v>
       </c>
       <c r="Y11" s="2" t="s">
         <v>2</v>
@@ -1582,37 +1433,37 @@
         <v>0</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AG11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AJ11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL11" s="2" t="s">
         <v>2</v>
@@ -1621,35 +1472,19 @@
         <v>0</v>
       </c>
       <c r="AN11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS11" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
       <c r="AT11" s="1"/>
       <c r="AU11" s="1"/>
       <c r="AV11" s="1"/>
-      <c r="AW11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY11" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
       <c r="AZ11" s="1"/>
       <c r="BA11" s="1"/>
       <c r="BB11" s="1"/>
@@ -1664,19 +1499,19 @@
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>0</v>
@@ -1691,10 +1526,10 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>2</v>
@@ -1703,23 +1538,27 @@
         <v>0</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R12">
         <f t="shared" si="0"/>
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>119</v>
       </c>
       <c r="T12">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U12">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>221</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="4"/>
+        <v>119,119,93,221,</v>
       </c>
       <c r="Y12" s="2" t="s">
         <v>2</v>
@@ -1728,19 +1567,19 @@
         <v>0</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF12" s="2" t="s">
         <v>0</v>
@@ -1755,10 +1594,10 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL12" s="2" t="s">
         <v>2</v>
@@ -1767,23 +1606,13 @@
         <v>0</v>
       </c>
       <c r="AN12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS12" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
       <c r="AT12" s="1"/>
       <c r="AU12" s="1"/>
       <c r="AV12" s="1"/>
@@ -1804,19 +1633,19 @@
         <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>0</v>
@@ -1831,33 +1660,39 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="O13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="T13">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U13">
         <f t="shared" si="3"/>
-        <v>69</v>
+        <v>221</v>
+      </c>
+      <c r="W13" t="str">
+        <f t="shared" si="4"/>
+        <v>119,119,93,221,</v>
       </c>
       <c r="Y13" s="2" t="s">
         <v>2</v>
@@ -1866,19 +1701,19 @@
         <v>0</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF13" s="2" t="s">
         <v>0</v>
@@ -1893,43 +1728,31 @@
         <v>0</v>
       </c>
       <c r="AJ13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL13" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL13" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AM13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AR13" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
       <c r="AS13" s="1"/>
       <c r="AT13" s="1"/>
       <c r="AU13" s="1"/>
       <c r="AV13" s="1"/>
-      <c r="AW13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY13" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
+      <c r="AY13" s="1"/>
       <c r="AZ13" s="1"/>
       <c r="BA13" s="1"/>
       <c r="BB13" s="1"/>
@@ -1944,17 +1767,19 @@
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>0</v>
@@ -1969,31 +1794,39 @@
         <v>0</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="P14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="R14">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U14">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>221</v>
+      </c>
+      <c r="W14" t="str">
+        <f t="shared" si="4"/>
+        <v>119,119,93,221,</v>
       </c>
       <c r="Y14" s="2" t="s">
         <v>2</v>
@@ -2002,17 +1835,19 @@
         <v>0</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC14" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AD14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF14" s="2" t="s">
         <v>0</v>
@@ -2027,44 +1862,32 @@
         <v>0</v>
       </c>
       <c r="AJ14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL14" s="2"/>
-      <c r="AM14" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AN14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
       <c r="AR14" s="1"/>
       <c r="AS14" s="1"/>
       <c r="AT14" s="1"/>
       <c r="AU14" s="1"/>
-      <c r="AV14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ14" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
       <c r="BA14" s="1"/>
       <c r="BB14" s="1"/>
       <c r="BC14" s="1"/>
@@ -2078,17 +1901,19 @@
         <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>0</v>
@@ -2103,31 +1928,39 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="P15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="R15">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="T15">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U15">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>221</v>
+      </c>
+      <c r="W15" t="str">
+        <f t="shared" si="4"/>
+        <v>119,119,93,221,</v>
       </c>
       <c r="Y15" s="2" t="s">
         <v>2</v>
@@ -2136,17 +1969,19 @@
         <v>0</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC15" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AD15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF15" s="2" t="s">
         <v>0</v>
@@ -2161,44 +1996,32 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL15" s="2"/>
-      <c r="AM15" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM15" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AN15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
       <c r="AR15" s="1"/>
       <c r="AS15" s="1"/>
       <c r="AT15" s="1"/>
       <c r="AU15" s="1"/>
-      <c r="AV15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ15" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
       <c r="BA15" s="1"/>
       <c r="BB15" s="1"/>
       <c r="BC15" s="1"/>
@@ -2212,17 +2035,19 @@
         <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>0</v>
@@ -2237,33 +2062,39 @@
         <v>0</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="2"/>
+      <c r="O16" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="P16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="R16">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="S16">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="T16">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U16">
         <f t="shared" si="3"/>
-        <v>81</v>
+        <v>221</v>
+      </c>
+      <c r="W16" t="str">
+        <f t="shared" si="4"/>
+        <v>119,119,93,221,</v>
       </c>
       <c r="Y16" s="2" t="s">
         <v>2</v>
@@ -2272,17 +2103,19 @@
         <v>0</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC16" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AD16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF16" s="2" t="s">
         <v>0</v>
@@ -2297,48 +2130,32 @@
         <v>0</v>
       </c>
       <c r="AJ16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AM16" s="2"/>
+      <c r="AM16" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AN16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AR16" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
       <c r="AS16" s="1"/>
       <c r="AT16" s="1"/>
       <c r="AU16" s="1"/>
-      <c r="AV16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ16" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
       <c r="BA16" s="1"/>
       <c r="BB16" s="1"/>
       <c r="BC16" s="1"/>
@@ -2352,17 +2169,19 @@
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F17" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>0</v>
@@ -2377,35 +2196,39 @@
         <v>0</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="R17">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="T17">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U17">
         <f t="shared" si="3"/>
-        <v>245</v>
+        <v>221</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="4"/>
+        <v>119,119,93,221,</v>
       </c>
       <c r="Y17" s="2" t="s">
         <v>2</v>
@@ -2414,17 +2237,19 @@
         <v>0</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC17" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AD17" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF17" s="2" t="s">
         <v>0</v>
@@ -2439,65 +2264,43 @@
         <v>0</v>
       </c>
       <c r="AJ17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AL17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM17" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS17" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
       <c r="AT17" s="1"/>
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
-      <c r="AW17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AZ17" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="1"/>
       <c r="BA17" s="1"/>
       <c r="BB17" s="1"/>
       <c r="BC17" s="1"/>
       <c r="BD17" s="1"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>2</v>
       </c>
@@ -2505,57 +2308,49 @@
       <c r="F18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="N18" s="2"/>
       <c r="O18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="P18" s="2"/>
       <c r="R18">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="T18">
         <f t="shared" si="2"/>
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="U18">
         <f t="shared" si="3"/>
-        <v>244</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="W18" t="str">
+        <f t="shared" si="4"/>
+        <v>17,17,4,68,</v>
+      </c>
+      <c r="Y18" s="2"/>
       <c r="Z18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AA18" s="2"/>
       <c r="AB18" s="2" t="s">
         <v>2</v>
       </c>
@@ -2563,47 +2358,29 @@
       <c r="AD18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AE18" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="AE18" s="2"/>
       <c r="AF18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AJ18" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="AJ18" s="2"/>
       <c r="AK18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL18" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AL18" s="2"/>
       <c r="AM18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AN18" s="2"/>
-      <c r="AO18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS18" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="1"/>
+      <c r="AS18" s="1"/>
       <c r="AT18" s="1"/>
       <c r="AU18" s="1"/>
       <c r="AV18" s="1"/>
@@ -2618,91 +2395,61 @@
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="R19">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T19">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>0</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" si="4"/>
+        <v>0,0,0,0,</v>
       </c>
       <c r="Y19" s="2"/>
-      <c r="Z19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA19" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
-      <c r="AE19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF19" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
-      <c r="AJ19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL19" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ19" s="2"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="1"/>
-      <c r="AP19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AR19" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AP19" s="1"/>
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="1"/>
       <c r="AS19" s="1"/>
       <c r="AT19" s="1"/>
       <c r="AU19" s="1"/>
@@ -2748,6 +2495,10 @@
       <c r="U20">
         <f t="shared" si="3"/>
         <v>0</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="4"/>
+        <v>0,0,0,0,</v>
       </c>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
@@ -2800,20 +2551,24 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="R21">
-        <f t="shared" ref="R21" si="4">IF(A21="o",64,0)+IF(A21="x",192,0)+IF(B21="o",16,0)+IF(B21="x",48,0)+IF(C21="o",4,0)+IF(C21="x",12,0)+IF(D21="o",1,0)+IF(D21="x",3,0)</f>
+        <f t="shared" ref="R21" si="5">IF(A21="o",64,0)+IF(A21="x",192,0)+IF(B21="o",16,0)+IF(B21="x",48,0)+IF(C21="o",4,0)+IF(C21="x",12,0)+IF(D21="o",1,0)+IF(D21="x",3,0)</f>
         <v>0</v>
       </c>
       <c r="S21">
-        <f t="shared" ref="S21" si="5">IF(E21="o",64,0)+IF(E21="x",192,0)+IF(F21="o",16,0)+IF(F21="x",48,0)+IF(G21="o",4,0)+IF(G21="x",12,0)+IF(H21="o",1,0)+IF(H21="x",3,0)</f>
+        <f t="shared" ref="S21" si="6">IF(E21="o",64,0)+IF(E21="x",192,0)+IF(F21="o",16,0)+IF(F21="x",48,0)+IF(G21="o",4,0)+IF(G21="x",12,0)+IF(H21="o",1,0)+IF(H21="x",3,0)</f>
         <v>0</v>
       </c>
       <c r="T21">
-        <f t="shared" ref="T21" si="6">IF(I21="o",64,0)+IF(I21="x",192,0)+IF(J21="o",16,0)+IF(J21="x",48,0)+IF(K21="o",4,0)+IF(K21="x",12,0)+IF(L21="o",1,0)+IF(L21="x",3,0)</f>
+        <f t="shared" ref="T21" si="7">IF(I21="o",64,0)+IF(I21="x",192,0)+IF(J21="o",16,0)+IF(J21="x",48,0)+IF(K21="o",4,0)+IF(K21="x",12,0)+IF(L21="o",1,0)+IF(L21="x",3,0)</f>
         <v>0</v>
       </c>
       <c r="U21">
-        <f t="shared" ref="U21" si="7">IF(M21="o",64,0)+IF(M21="x",192,0)+IF(N21="o",16,0)+IF(N21="x",48,0)+IF(O21="o",4,0)+IF(O21="x",12,0)+IF(P21="o",1,0)+IF(P21="x",3,0)</f>
-        <v>0</v>
+        <f t="shared" ref="U21" si="8">IF(M21="o",64,0)+IF(M21="x",192,0)+IF(N21="o",16,0)+IF(N21="x",48,0)+IF(O21="o",4,0)+IF(O21="x",12,0)+IF(P21="o",1,0)+IF(P21="x",3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W21" t="str">
+        <f t="shared" si="4"/>
+        <v>0,0,0,0,</v>
       </c>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
@@ -2848,6 +2603,21 @@
       <c r="BC21" s="1"/>
       <c r="BD21" s="1"/>
     </row>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="W22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="W23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="W24" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
@@ -2881,6 +2651,10 @@
         <f>IF(M25="o",64,0)+IF(M25="x",192,0)+IF(N25="o",16,0)+IF(N25="x",48,0)+IF(O25="o",4,0)+IF(O25="x",12,0)+IF(P25="o",1,0)+IF(P25="x",3,0)</f>
         <v>0</v>
       </c>
+      <c r="W25" t="str">
+        <f t="shared" si="4"/>
+        <v>0,0,0,0,</v>
+      </c>
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -2900,20 +2674,24 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="R26">
-        <f t="shared" ref="R26:R44" si="8">IF(A26="o",64,0)+IF(A26="x",192,0)+IF(B26="o",16,0)+IF(B26="x",48,0)+IF(C26="o",4,0)+IF(C26="x",12,0)+IF(D26="o",1,0)+IF(D26="x",3,0)</f>
+        <f t="shared" ref="R26:R44" si="9">IF(A26="o",64,0)+IF(A26="x",192,0)+IF(B26="o",16,0)+IF(B26="x",48,0)+IF(C26="o",4,0)+IF(C26="x",12,0)+IF(D26="o",1,0)+IF(D26="x",3,0)</f>
         <v>0</v>
       </c>
       <c r="S26">
-        <f t="shared" ref="S26:S44" si="9">IF(E26="o",64,0)+IF(E26="x",192,0)+IF(F26="o",16,0)+IF(F26="x",48,0)+IF(G26="o",4,0)+IF(G26="x",12,0)+IF(H26="o",1,0)+IF(H26="x",3,0)</f>
+        <f t="shared" ref="S26:S44" si="10">IF(E26="o",64,0)+IF(E26="x",192,0)+IF(F26="o",16,0)+IF(F26="x",48,0)+IF(G26="o",4,0)+IF(G26="x",12,0)+IF(H26="o",1,0)+IF(H26="x",3,0)</f>
         <v>0</v>
       </c>
       <c r="T26">
-        <f t="shared" ref="T26:T44" si="10">IF(I26="o",64,0)+IF(I26="x",192,0)+IF(J26="o",16,0)+IF(J26="x",48,0)+IF(K26="o",4,0)+IF(K26="x",12,0)+IF(L26="o",1,0)+IF(L26="x",3,0)</f>
+        <f t="shared" ref="T26:T44" si="11">IF(I26="o",64,0)+IF(I26="x",192,0)+IF(J26="o",16,0)+IF(J26="x",48,0)+IF(K26="o",4,0)+IF(K26="x",12,0)+IF(L26="o",1,0)+IF(L26="x",3,0)</f>
         <v>0</v>
       </c>
       <c r="U26">
-        <f t="shared" ref="U26:U44" si="11">IF(M26="o",64,0)+IF(M26="x",192,0)+IF(N26="o",16,0)+IF(N26="x",48,0)+IF(O26="o",4,0)+IF(O26="x",12,0)+IF(P26="o",1,0)+IF(P26="x",3,0)</f>
-        <v>0</v>
+        <f t="shared" ref="U26:U44" si="12">IF(M26="o",64,0)+IF(M26="x",192,0)+IF(N26="o",16,0)+IF(N26="x",48,0)+IF(O26="o",4,0)+IF(O26="x",12,0)+IF(P26="o",1,0)+IF(P26="x",3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W26" t="str">
+        <f t="shared" si="4"/>
+        <v>0,0,0,0,</v>
       </c>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.25">
@@ -2938,20 +2716,24 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="R27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>80</v>
       </c>
       <c r="S27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U27">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W27" t="str">
+        <f t="shared" si="4"/>
+        <v>80,0,0,0,</v>
       </c>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.25">
@@ -2978,20 +2760,24 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="R28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>244</v>
       </c>
       <c r="S28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U28">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W28" t="str">
+        <f t="shared" si="4"/>
+        <v>244,0,0,0,</v>
       </c>
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.25">
@@ -3018,20 +2804,24 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="R29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>244</v>
       </c>
       <c r="S29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U29">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W29" t="str">
+        <f t="shared" si="4"/>
+        <v>244,0,0,0,</v>
       </c>
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.25">
@@ -3064,20 +2854,24 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="R30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>244</v>
       </c>
       <c r="S30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>84</v>
       </c>
       <c r="U30">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W30" t="str">
+        <f t="shared" si="4"/>
+        <v>244,0,84,0,</v>
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.25">
@@ -3114,20 +2908,24 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="R31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>244</v>
       </c>
       <c r="S31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="T31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>253</v>
       </c>
       <c r="U31">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W31" t="str">
+        <f t="shared" si="4"/>
+        <v>244,1,253,0,</v>
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.25">
@@ -3164,23 +2962,27 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="R32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>244</v>
       </c>
       <c r="S32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="T32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>253</v>
       </c>
       <c r="U32">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W32" t="str">
+        <f t="shared" si="4"/>
+        <v>244,1,253,0,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -3216,23 +3018,27 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="R33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>245</v>
       </c>
       <c r="S33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="T33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>253</v>
       </c>
       <c r="U33">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W33" t="str">
+        <f t="shared" si="4"/>
+        <v>245,1,253,0,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -3266,23 +3072,27 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="R34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>255</v>
       </c>
       <c r="S34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="T34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>84</v>
       </c>
       <c r="U34">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W34" t="str">
+        <f t="shared" si="4"/>
+        <v>255,64,84,0,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -3310,23 +3120,27 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="R35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>255</v>
       </c>
       <c r="S35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="T35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U35">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W35" t="str">
+        <f t="shared" si="4"/>
+        <v>255,64,0,0,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -3358,23 +3172,27 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="R36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>245</v>
       </c>
       <c r="S36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>84</v>
       </c>
       <c r="U36">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W36" t="str">
+        <f t="shared" si="4"/>
+        <v>245,0,84,0,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -3408,23 +3226,27 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="R37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>244</v>
       </c>
       <c r="S37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="T37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>253</v>
       </c>
       <c r="U37">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W37" t="str">
+        <f t="shared" si="4"/>
+        <v>244,1,253,0,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -3458,23 +3280,27 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="R38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>244</v>
       </c>
       <c r="S38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="T38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>253</v>
       </c>
       <c r="U38">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W38" t="str">
+        <f t="shared" si="4"/>
+        <v>244,1,253,0,</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -3510,23 +3336,27 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="R39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>245</v>
       </c>
       <c r="S39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="T39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>253</v>
       </c>
       <c r="U39">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W39" t="str">
+        <f t="shared" si="4"/>
+        <v>245,1,253,0,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -3562,23 +3392,27 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="R40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>255</v>
       </c>
       <c r="S40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="T40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>85</v>
       </c>
       <c r="U40">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W40" t="str">
+        <f t="shared" si="4"/>
+        <v>255,64,85,0,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
@@ -3606,23 +3440,27 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="R41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>127</v>
       </c>
       <c r="S41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="T41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U41">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W41" t="str">
+        <f t="shared" si="4"/>
+        <v>127,64,0,0,</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>2</v>
@@ -3646,23 +3484,27 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="R42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="S42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U42">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W42" t="str">
+        <f t="shared" si="4"/>
+        <v>21,0,0,0,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3680,23 +3522,27 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="R43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U43">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W43" t="str">
+        <f t="shared" si="4"/>
+        <v>0,0,0,0,</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3714,20 +3560,24 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="R44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U44">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W44" t="str">
+        <f t="shared" si="4"/>
+        <v>0,0,0,0,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Center marker added Ground speed added
</commit_message>
<xml_diff>
--- a/tools/16x20char_designer.xlsx
+++ b/tools/16x20char_designer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\00GIT\OSDeluxe\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B0C0D9-B644-4D28-ABE1-C929C83846E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68E07A0-EB59-4558-8A20-27DF42FD1B8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="9120" xr2:uid="{7204D92D-006B-4887-9E42-7235DD687936}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="4">
   <si>
     <t>x</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>o</t>
+  </si>
+  <si>
+    <t>oo</t>
   </si>
 </sst>
 </file>
@@ -95,10 +98,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -418,7 +422,7 @@
   <dimension ref="A1:BD44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2:W21"/>
+      <selection activeCell="W25" sqref="W25:W44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,13 +489,21 @@
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -502,11 +514,11 @@
       <c r="P2" s="2"/>
       <c r="R2">
         <f>IF(A2="o",64,0)+IF(A2="x",192,0)+IF(B2="o",16,0)+IF(B2="x",48,0)+IF(C2="o",4,0)+IF(C2="x",12,0)+IF(D2="o",1,0)+IF(D2="x",3,0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S2">
         <f>IF(E2="o",64,0)+IF(E2="x",192,0)+IF(F2="o",16,0)+IF(F2="x",48,0)+IF(G2="o",4,0)+IF(G2="x",12,0)+IF(H2="o",1,0)+IF(H2="x",3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T2">
         <f>IF(I2="o",64,0)+IF(I2="x",192,0)+IF(J2="o",16,0)+IF(J2="x",48,0)+IF(K2="o",4,0)+IF(K2="x",12,0)+IF(L2="o",1,0)+IF(L2="x",3,0)</f>
@@ -518,16 +530,24 @@
       </c>
       <c r="W2" t="str">
         <f>_xlfn.CONCAT(R2,",",S2,",",T2,",",U2,",")</f>
-        <v>0,0,0,0,</v>
+        <v>20,5,0,0,</v>
       </c>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
+      <c r="Z2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
+      <c r="AE2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -539,9 +559,15 @@
       <c r="AO2" s="1"/>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
+      <c r="AR2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
@@ -554,15 +580,31 @@
       <c r="BD2" s="1"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -575,15 +617,15 @@
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R20" si="0">IF(A3="o",64,0)+IF(A3="x",192,0)+IF(B3="o",16,0)+IF(B3="x",48,0)+IF(C3="o",4,0)+IF(C3="x",12,0)+IF(D3="o",1,0)+IF(D3="x",3,0)</f>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S20" si="1">IF(E3="o",64,0)+IF(E3="x",192,0)+IF(F3="o",16,0)+IF(F3="x",48,0)+IF(G3="o",4,0)+IF(G3="x",12,0)+IF(H3="o",1,0)+IF(H3="x",3,0)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T20" si="2">IF(I3="o",64,0)+IF(I3="x",192,0)+IF(J3="o",16,0)+IF(J3="x",48,0)+IF(K3="o",4,0)+IF(K3="x",12,0)+IF(L3="o",1,0)+IF(L3="x",3,0)</f>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U20" si="3">IF(M3="o",64,0)+IF(M3="x",192,0)+IF(N3="o",16,0)+IF(N3="x",48,0)+IF(O3="o",4,0)+IF(O3="x",12,0)+IF(P3="o",1,0)+IF(P3="x",3,0)</f>
@@ -591,17 +633,33 @@
       </c>
       <c r="W3" t="str">
         <f t="shared" ref="W3:W44" si="4">_xlfn.CONCAT(R3,",",S3,",",T3,",",U3,",")</f>
-        <v>0,0,0,0,</v>
-      </c>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
+        <v>125,31,64,0,</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
+      <c r="AD3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
@@ -612,10 +670,18 @@
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
+      <c r="AR3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
@@ -627,25 +693,35 @@
       <c r="BD3" s="1"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="I4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -654,53 +730,71 @@
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="W4" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,80,64,</v>
-      </c>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
+        <v>125,31,64,0,</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
+      <c r="AD4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AG4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AH4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
-      <c r="AK4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
-      <c r="AT4" s="1"/>
-      <c r="AU4" s="1"/>
+      <c r="AR4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
@@ -712,34 +806,36 @@
       <c r="BD4" s="1"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="H5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" t="s">
@@ -747,61 +843,71 @@
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="S5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>245</v>
+        <v>64</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="4"/>
-        <v>0,1,245,208,</v>
-      </c>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
+        <v>125,31,64,0,</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
+      <c r="AD5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AF5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="1"/>
-      <c r="AT5" s="1"/>
-      <c r="AU5" s="1"/>
+      <c r="AR5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
       <c r="AX5" s="1"/>
@@ -813,100 +919,112 @@
       <c r="BD5" s="1"/>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="P6" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="Q6" t="s">
         <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>125</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="4"/>
-        <v>0,7,93,208,</v>
-      </c>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
+        <v>125,125,0,0,</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AE6" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
-      <c r="AN6" s="2"/>
+      <c r="AN6" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1"/>
-      <c r="AT6" s="1"/>
-      <c r="AU6" s="1"/>
+      <c r="AR6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
@@ -918,100 +1036,128 @@
       <c r="BD6" s="1"/>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>125</v>
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>208</v>
+        <v>65</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="4"/>
-        <v>0,7,93,208,</v>
-      </c>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
+        <v>125,125,1,65,</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AE7" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI7" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
       <c r="AJ7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
-      <c r="AO7" s="1"/>
+      <c r="AN7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
-      <c r="AR7" s="1"/>
-      <c r="AS7" s="1"/>
-      <c r="AT7" s="1"/>
-      <c r="AU7" s="1"/>
-      <c r="AV7" s="1"/>
-      <c r="AW7" s="1"/>
-      <c r="AX7" s="1"/>
+      <c r="AR7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX7" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
@@ -1020,29 +1166,35 @@
       <c r="BD7" s="1"/>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="G8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>0</v>
@@ -1050,51 +1202,61 @@
       <c r="N8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="O8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="S8">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="4"/>
-        <v>0,7,93,208,</v>
-      </c>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
+        <v>125,116,7,215,</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AE8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AF8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
       <c r="AI8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>0</v>
@@ -1102,19 +1264,43 @@
       <c r="AL8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2"/>
-      <c r="AO8" s="1"/>
-      <c r="AP8" s="1"/>
+      <c r="AM8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AQ8" s="1"/>
-      <c r="AR8" s="1"/>
-      <c r="AS8" s="1"/>
-      <c r="AT8" s="1"/>
-      <c r="AU8" s="1"/>
-      <c r="AV8" s="1"/>
-      <c r="AW8" s="1"/>
-      <c r="AX8" s="1"/>
-      <c r="AY8" s="1"/>
+      <c r="AR8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AZ8" s="1"/>
       <c r="BA8" s="1"/>
       <c r="BB8" s="1"/>
@@ -1122,25 +1308,27 @@
       <c r="BD8" s="1"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1148,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>0</v>
@@ -1156,47 +1344,53 @@
       <c r="N9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="O9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>208</v>
       </c>
       <c r="T9">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="4"/>
-        <v>4,71,93,208,</v>
-      </c>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
+        <v>127,208,31,215,</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AA9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB9" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AC9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
       <c r="AH9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1204,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="AJ9" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>0</v>
@@ -1212,50 +1406,78 @@
       <c r="AL9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AM9" s="2"/>
-      <c r="AN9" s="2"/>
-      <c r="AO9" s="1"/>
-      <c r="AP9" s="1"/>
-      <c r="AQ9" s="1"/>
-      <c r="AR9" s="1"/>
-      <c r="AS9" s="1"/>
-      <c r="AT9" s="1"/>
-      <c r="AU9" s="1"/>
-      <c r="AV9" s="1"/>
-      <c r="AW9" s="1"/>
-      <c r="AX9" s="1"/>
-      <c r="AY9" s="1"/>
-      <c r="AZ9" s="1"/>
+      <c r="AM9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BA9" s="1"/>
       <c r="BB9" s="1"/>
       <c r="BC9" s="1"/>
       <c r="BD9" s="1"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="B10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>0</v>
@@ -1267,59 +1489,61 @@
         <v>2</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P10" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="R10">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>215</v>
+        <v>244</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>253</v>
+        <v>125</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="4"/>
-        <v>29,215,253,244,</v>
-      </c>
-      <c r="Y10" s="2"/>
+        <v>127,244,125,125,</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="Z10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AF10" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="AF10" s="2"/>
       <c r="AG10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH10" s="2" t="s">
         <v>0</v>
@@ -1331,27 +1555,53 @@
         <v>2</v>
       </c>
       <c r="AK10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AM10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN10" s="2"/>
-      <c r="AO10" s="1"/>
-      <c r="AP10" s="1"/>
-      <c r="AQ10" s="1"/>
-      <c r="AR10" s="1"/>
-      <c r="AS10" s="1"/>
-      <c r="AT10" s="1"/>
-      <c r="AU10" s="1"/>
-      <c r="AV10" s="1"/>
-      <c r="AW10" s="1"/>
-      <c r="AX10" s="1"/>
-      <c r="AY10" s="1"/>
-      <c r="AZ10" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BA10" s="1"/>
       <c r="BB10" s="1"/>
       <c r="BC10" s="1"/>
@@ -1365,10 +1615,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>2</v>
@@ -1377,13 +1627,13 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>0</v>
@@ -1395,10 +1645,10 @@
         <v>2</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>0</v>
@@ -1408,23 +1658,23 @@
       </c>
       <c r="R11">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="T11">
         <f t="shared" si="2"/>
-        <v>253</v>
+        <v>125</v>
       </c>
       <c r="U11">
         <f t="shared" si="3"/>
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="4"/>
-        <v>119,119,253,221,</v>
+        <v>125,125,125,125,</v>
       </c>
       <c r="Y11" s="2" t="s">
         <v>2</v>
@@ -1433,10 +1683,10 @@
         <v>0</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC11" s="2" t="s">
         <v>2</v>
@@ -1445,13 +1695,13 @@
         <v>0</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH11" s="2" t="s">
         <v>0</v>
@@ -1463,10 +1713,10 @@
         <v>2</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM11" s="2" t="s">
         <v>0</v>
@@ -1474,18 +1724,40 @@
       <c r="AN11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO11" s="1"/>
-      <c r="AP11" s="1"/>
-      <c r="AQ11" s="1"/>
-      <c r="AR11" s="1"/>
-      <c r="AS11" s="1"/>
-      <c r="AT11" s="1"/>
-      <c r="AU11" s="1"/>
+      <c r="AO11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV11" s="1"/>
-      <c r="AW11" s="1"/>
-      <c r="AX11" s="1"/>
-      <c r="AY11" s="1"/>
-      <c r="AZ11" s="1"/>
+      <c r="AW11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ11" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BA11" s="1"/>
       <c r="BB11" s="1"/>
       <c r="BC11" s="1"/>
@@ -1499,10 +1771,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
@@ -1511,16 +1783,16 @@
         <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>0</v>
@@ -1529,10 +1801,10 @@
         <v>2</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>0</v>
@@ -1542,23 +1814,23 @@
       </c>
       <c r="R12">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="T12">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="U12">
         <f t="shared" si="3"/>
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="4"/>
-        <v>119,119,93,221,</v>
+        <v>125,125,125,125,</v>
       </c>
       <c r="Y12" s="2" t="s">
         <v>2</v>
@@ -1567,10 +1839,10 @@
         <v>0</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC12" s="2" t="s">
         <v>2</v>
@@ -1579,16 +1851,16 @@
         <v>0</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI12" s="2" t="s">
         <v>0</v>
@@ -1597,10 +1869,10 @@
         <v>2</v>
       </c>
       <c r="AK12" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM12" s="2" t="s">
         <v>0</v>
@@ -1608,18 +1880,40 @@
       <c r="AN12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO12" s="1"/>
-      <c r="AP12" s="1"/>
-      <c r="AQ12" s="1"/>
-      <c r="AR12" s="1"/>
-      <c r="AS12" s="1"/>
-      <c r="AT12" s="1"/>
-      <c r="AU12" s="1"/>
+      <c r="AO12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV12" s="1"/>
-      <c r="AW12" s="1"/>
-      <c r="AX12" s="1"/>
-      <c r="AY12" s="1"/>
-      <c r="AZ12" s="1"/>
+      <c r="AW12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ12" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BA12" s="1"/>
       <c r="BB12" s="1"/>
       <c r="BC12" s="1"/>
@@ -1633,19 +1927,17 @@
         <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>0</v>
@@ -1654,7 +1946,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>0</v>
@@ -1663,10 +1955,10 @@
         <v>2</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>0</v>
@@ -1676,23 +1968,23 @@
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>31</v>
       </c>
       <c r="T13">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="U13">
         <f t="shared" si="3"/>
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="4"/>
-        <v>119,119,93,221,</v>
+        <v>125,31,125,125,</v>
       </c>
       <c r="Y13" s="2" t="s">
         <v>2</v>
@@ -1701,19 +1993,17 @@
         <v>0</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AC13" s="2"/>
       <c r="AD13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF13" s="2" t="s">
         <v>0</v>
@@ -1722,7 +2012,7 @@
         <v>2</v>
       </c>
       <c r="AH13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI13" s="2" t="s">
         <v>0</v>
@@ -1731,10 +2021,10 @@
         <v>2</v>
       </c>
       <c r="AK13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM13" s="2" t="s">
         <v>0</v>
@@ -1742,18 +2032,40 @@
       <c r="AN13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO13" s="1"/>
-      <c r="AP13" s="1"/>
-      <c r="AQ13" s="1"/>
-      <c r="AR13" s="1"/>
-      <c r="AS13" s="1"/>
-      <c r="AT13" s="1"/>
-      <c r="AU13" s="1"/>
+      <c r="AO13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV13" s="1"/>
-      <c r="AW13" s="1"/>
-      <c r="AX13" s="1"/>
-      <c r="AY13" s="1"/>
-      <c r="AZ13" s="1"/>
+      <c r="AW13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ13" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BA13" s="1"/>
       <c r="BB13" s="1"/>
       <c r="BC13" s="1"/>
@@ -1767,19 +2079,17 @@
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>0</v>
@@ -1788,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>0</v>
@@ -1797,10 +2107,10 @@
         <v>2</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>0</v>
@@ -1810,23 +2120,23 @@
       </c>
       <c r="R14">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>31</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="U14">
         <f t="shared" si="3"/>
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="W14" t="str">
         <f t="shared" si="4"/>
-        <v>119,119,93,221,</v>
+        <v>125,31,125,125,</v>
       </c>
       <c r="Y14" s="2" t="s">
         <v>2</v>
@@ -1835,19 +2145,17 @@
         <v>0</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AC14" s="2"/>
       <c r="AD14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="2" t="s">
         <v>0</v>
@@ -1856,7 +2164,7 @@
         <v>2</v>
       </c>
       <c r="AH14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI14" s="2" t="s">
         <v>0</v>
@@ -1865,10 +2173,10 @@
         <v>2</v>
       </c>
       <c r="AK14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM14" s="2" t="s">
         <v>0</v>
@@ -1876,18 +2184,40 @@
       <c r="AN14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO14" s="1"/>
-      <c r="AP14" s="1"/>
-      <c r="AQ14" s="1"/>
-      <c r="AR14" s="1"/>
-      <c r="AS14" s="1"/>
-      <c r="AT14" s="1"/>
-      <c r="AU14" s="1"/>
+      <c r="AO14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV14" s="1"/>
-      <c r="AW14" s="1"/>
-      <c r="AX14" s="1"/>
-      <c r="AY14" s="1"/>
-      <c r="AZ14" s="1"/>
+      <c r="AW14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ14" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BA14" s="1"/>
       <c r="BB14" s="1"/>
       <c r="BC14" s="1"/>
@@ -1901,19 +2231,17 @@
         <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>0</v>
@@ -1922,7 +2250,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>0</v>
@@ -1931,10 +2259,10 @@
         <v>2</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>0</v>
@@ -1944,23 +2272,23 @@
       </c>
       <c r="R15">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>31</v>
       </c>
       <c r="T15">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="U15">
         <f t="shared" si="3"/>
-        <v>221</v>
+        <v>61</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="4"/>
-        <v>119,119,93,221,</v>
+        <v>125,31,125,61,</v>
       </c>
       <c r="Y15" s="2" t="s">
         <v>2</v>
@@ -1969,19 +2297,17 @@
         <v>0</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AC15" s="2"/>
       <c r="AD15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF15" s="2" t="s">
         <v>0</v>
@@ -1990,7 +2316,7 @@
         <v>2</v>
       </c>
       <c r="AH15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI15" s="2" t="s">
         <v>0</v>
@@ -1999,10 +2325,10 @@
         <v>2</v>
       </c>
       <c r="AK15" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM15" s="2" t="s">
         <v>0</v>
@@ -2010,18 +2336,40 @@
       <c r="AN15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO15" s="1"/>
-      <c r="AP15" s="1"/>
-      <c r="AQ15" s="1"/>
-      <c r="AR15" s="1"/>
-      <c r="AS15" s="1"/>
-      <c r="AT15" s="1"/>
-      <c r="AU15" s="1"/>
+      <c r="AO15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU15" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV15" s="1"/>
-      <c r="AW15" s="1"/>
-      <c r="AX15" s="1"/>
-      <c r="AY15" s="1"/>
-      <c r="AZ15" s="1"/>
+      <c r="AW15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ15" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BA15" s="1"/>
       <c r="BB15" s="1"/>
       <c r="BC15" s="1"/>
@@ -2035,19 +2383,17 @@
         <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>0</v>
@@ -2056,7 +2402,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>0</v>
@@ -2065,10 +2411,10 @@
         <v>2</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>0</v>
@@ -2078,23 +2424,23 @@
       </c>
       <c r="R16">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="S16">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>31</v>
       </c>
       <c r="T16">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="U16">
         <f t="shared" si="3"/>
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="4"/>
-        <v>119,119,93,221,</v>
+        <v>125,31,125,125,</v>
       </c>
       <c r="Y16" s="2" t="s">
         <v>2</v>
@@ -2103,19 +2449,17 @@
         <v>0</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AC16" s="2"/>
       <c r="AD16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF16" s="2" t="s">
         <v>0</v>
@@ -2124,7 +2468,7 @@
         <v>2</v>
       </c>
       <c r="AH16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI16" s="2" t="s">
         <v>0</v>
@@ -2133,10 +2477,10 @@
         <v>2</v>
       </c>
       <c r="AK16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM16" s="2" t="s">
         <v>0</v>
@@ -2144,151 +2488,157 @@
       <c r="AN16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AO16" s="1"/>
-      <c r="AP16" s="1"/>
-      <c r="AQ16" s="1"/>
-      <c r="AR16" s="1"/>
-      <c r="AS16" s="1"/>
-      <c r="AT16" s="1"/>
-      <c r="AU16" s="1"/>
+      <c r="AO16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV16" s="1"/>
-      <c r="AW16" s="1"/>
-      <c r="AX16" s="1"/>
-      <c r="AY16" s="1"/>
-      <c r="AZ16" s="1"/>
+      <c r="AW16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ16" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BA16" s="1"/>
       <c r="BB16" s="1"/>
       <c r="BC16" s="1"/>
       <c r="BD16" s="1"/>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M17" s="2"/>
       <c r="N17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="P17" s="2"/>
       <c r="R17">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>5</v>
       </c>
       <c r="T17">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="U17">
         <f t="shared" si="3"/>
-        <v>221</v>
+        <v>20</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="4"/>
-        <v>119,119,93,221,</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>20,5,20,20,</v>
+      </c>
+      <c r="Y17" s="2"/>
       <c r="Z17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AB17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD17" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
       <c r="AE17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AF17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AG17" s="2"/>
       <c r="AH17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AI17" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK17" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AK17" s="2"/>
       <c r="AL17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AM17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN17" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AN17" s="2"/>
       <c r="AO17" s="1"/>
-      <c r="AP17" s="1"/>
-      <c r="AQ17" s="1"/>
+      <c r="AP17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ17" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AR17" s="1"/>
-      <c r="AS17" s="1"/>
-      <c r="AT17" s="1"/>
+      <c r="AS17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT17" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
-      <c r="AX17" s="1"/>
-      <c r="AY17" s="1"/>
+      <c r="AX17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY17" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AZ17" s="1"/>
       <c r="BA17" s="1"/>
       <c r="BB17" s="1"/>
@@ -2296,86 +2646,58 @@
       <c r="BD17" s="1"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
       <c r="R18">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T18">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U18">
         <f t="shared" si="3"/>
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="W18" t="str">
         <f t="shared" si="4"/>
-        <v>17,17,4,68,</v>
-      </c>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC18" s="2"/>
-      <c r="AD18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2"/>
-      <c r="AI18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL18" s="2"/>
-      <c r="AM18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN18" s="2"/>
+        <v>0,0,0,0,</v>
+      </c>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="3"/>
       <c r="AO18" s="1"/>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
@@ -2622,9 +2944,15 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2641,7 +2969,7 @@
       </c>
       <c r="S25">
         <f>IF(E25="o",64,0)+IF(E25="x",192,0)+IF(F25="o",16,0)+IF(F25="x",48,0)+IF(G25="o",4,0)+IF(G25="x",12,0)+IF(H25="o",1,0)+IF(H25="x",3,0)</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T25">
         <f>IF(I25="o",64,0)+IF(I25="x",192,0)+IF(J25="o",16,0)+IF(J25="x",48,0)+IF(K25="o",4,0)+IF(K25="x",12,0)+IF(L25="o",1,0)+IF(L25="x",3,0)</f>
@@ -2653,17 +2981,25 @@
       </c>
       <c r="W25" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,</v>
+        <v>0,80,0,0,</v>
       </c>
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2675,11 +3011,11 @@
       <c r="P26" s="1"/>
       <c r="R26">
         <f t="shared" ref="R26:R44" si="9">IF(A26="o",64,0)+IF(A26="x",192,0)+IF(B26="o",16,0)+IF(B26="x",48,0)+IF(C26="o",4,0)+IF(C26="x",12,0)+IF(D26="o",1,0)+IF(D26="x",3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26">
         <f t="shared" ref="S26:S44" si="10">IF(E26="o",64,0)+IF(E26="x",192,0)+IF(F26="o",16,0)+IF(F26="x",48,0)+IF(G26="o",4,0)+IF(G26="x",12,0)+IF(H26="o",1,0)+IF(H26="x",3,0)</f>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="T26">
         <f t="shared" ref="T26:T44" si="11">IF(I26="o",64,0)+IF(I26="x",192,0)+IF(J26="o",16,0)+IF(J26="x",48,0)+IF(K26="o",4,0)+IF(K26="x",12,0)+IF(L26="o",1,0)+IF(L26="x",3,0)</f>
@@ -2691,21 +3027,25 @@
       </c>
       <c r="W26" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,</v>
+        <v>1,244,0,0,</v>
       </c>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2717,11 +3057,11 @@
       <c r="P27" s="1"/>
       <c r="R27">
         <f t="shared" si="9"/>
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="S27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="T27">
         <f t="shared" si="11"/>
@@ -2733,23 +3073,25 @@
       </c>
       <c r="W27" t="str">
         <f t="shared" si="4"/>
-        <v>80,0,0,0,</v>
+        <v>1,244,0,0,</v>
       </c>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -2761,11 +3103,11 @@
       <c r="P28" s="1"/>
       <c r="R28">
         <f t="shared" si="9"/>
-        <v>244</v>
+        <v>1</v>
       </c>
       <c r="S28">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="T28">
         <f t="shared" si="11"/>
@@ -2777,23 +3119,25 @@
       </c>
       <c r="W28" t="str">
         <f t="shared" si="4"/>
-        <v>244,0,0,0,</v>
+        <v>1,244,0,0,</v>
       </c>
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -2805,11 +3149,11 @@
       <c r="P29" s="1"/>
       <c r="R29">
         <f t="shared" si="9"/>
-        <v>244</v>
+        <v>1</v>
       </c>
       <c r="S29">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="T29">
         <f t="shared" si="11"/>
@@ -2821,33 +3165,37 @@
       </c>
       <c r="W29" t="str">
         <f t="shared" si="4"/>
-        <v>244,0,0,0,</v>
+        <v>1,244,0,0,</v>
       </c>
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="I30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -2855,15 +3203,15 @@
       <c r="P30" s="1"/>
       <c r="R30">
         <f t="shared" si="9"/>
-        <v>244</v>
+        <v>65</v>
       </c>
       <c r="S30">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="T30">
         <f t="shared" si="11"/>
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="U30">
         <f t="shared" si="12"/>
@@ -2871,7 +3219,7 @@
       </c>
       <c r="W30" t="str">
         <f t="shared" si="4"/>
-        <v>244,0,84,0,</v>
+        <v>65,245,80,0,</v>
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.25">
@@ -2879,17 +3227,23 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="H31" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>0</v>
@@ -2898,26 +3252,24 @@
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="R31">
         <f t="shared" si="9"/>
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="S31">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="T31">
         <f t="shared" si="11"/>
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="U31">
         <f t="shared" si="12"/>
@@ -2925,7 +3277,7 @@
       </c>
       <c r="W31" t="str">
         <f t="shared" si="4"/>
-        <v>244,1,253,0,</v>
+        <v>209,255,244,0,</v>
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.25">
@@ -2938,12 +3290,20 @@
       <c r="C32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="H32" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>0</v>
@@ -2963,11 +3323,11 @@
       <c r="P32" s="1"/>
       <c r="R32">
         <f t="shared" si="9"/>
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="S32">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="T32">
         <f t="shared" si="11"/>
@@ -2979,30 +3339,36 @@
       </c>
       <c r="W32" t="str">
         <f t="shared" si="4"/>
-        <v>244,1,253,0,</v>
+        <v>245,255,253,0,</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>0</v>
@@ -3019,15 +3385,15 @@
       <c r="P33" s="1"/>
       <c r="R33">
         <f t="shared" si="9"/>
-        <v>245</v>
+        <v>125</v>
       </c>
       <c r="S33">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>245</v>
       </c>
       <c r="T33">
         <f t="shared" si="11"/>
-        <v>253</v>
+        <v>125</v>
       </c>
       <c r="U33">
         <f t="shared" si="12"/>
@@ -3035,12 +3401,12 @@
       </c>
       <c r="W33" t="str">
         <f t="shared" si="4"/>
-        <v>245,1,253,0,</v>
+        <v>125,245,125,0,</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -3049,39 +3415,45 @@
         <v>0</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L34" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="R34">
         <f t="shared" si="9"/>
-        <v>255</v>
+        <v>125</v>
       </c>
       <c r="S34">
         <f t="shared" si="10"/>
-        <v>64</v>
+        <v>244</v>
       </c>
       <c r="T34">
         <f t="shared" si="11"/>
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="U34">
         <f t="shared" si="12"/>
@@ -3089,12 +3461,12 @@
       </c>
       <c r="W34" t="str">
         <f t="shared" si="4"/>
-        <v>255,64,84,0,</v>
+        <v>125,244,125,0,</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>0</v>
@@ -3103,33 +3475,45 @@
         <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="R35">
         <f t="shared" si="9"/>
-        <v>255</v>
+        <v>125</v>
       </c>
       <c r="S35">
         <f t="shared" si="10"/>
-        <v>64</v>
+        <v>244</v>
       </c>
       <c r="T35">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="U35">
         <f t="shared" si="12"/>
@@ -3137,51 +3521,59 @@
       </c>
       <c r="W35" t="str">
         <f t="shared" si="4"/>
-        <v>255,64,0,0,</v>
+        <v>125,244,125,0,</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L36" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="R36">
         <f t="shared" si="9"/>
-        <v>245</v>
+        <v>125</v>
       </c>
       <c r="S36">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="T36">
         <f t="shared" si="11"/>
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="U36">
         <f t="shared" si="12"/>
@@ -3189,28 +3581,34 @@
       </c>
       <c r="W36" t="str">
         <f t="shared" si="4"/>
-        <v>245,0,84,0,</v>
+        <v>125,244,125,0,</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>0</v>
@@ -3227,15 +3625,15 @@
       <c r="P37" s="1"/>
       <c r="R37">
         <f t="shared" si="9"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="S37">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>244</v>
       </c>
       <c r="T37">
         <f t="shared" si="11"/>
-        <v>253</v>
+        <v>125</v>
       </c>
       <c r="U37">
         <f t="shared" si="12"/>
@@ -3243,28 +3641,34 @@
       </c>
       <c r="W37" t="str">
         <f t="shared" si="4"/>
-        <v>244,1,253,0,</v>
+        <v>125,244,125,0,</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>0</v>
@@ -3281,15 +3685,15 @@
       <c r="P38" s="1"/>
       <c r="R38">
         <f t="shared" si="9"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="S38">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>244</v>
       </c>
       <c r="T38">
         <f t="shared" si="11"/>
-        <v>253</v>
+        <v>125</v>
       </c>
       <c r="U38">
         <f t="shared" si="12"/>
@@ -3297,30 +3701,34 @@
       </c>
       <c r="W38" t="str">
         <f t="shared" si="4"/>
-        <v>244,1,253,0,</v>
+        <v>125,244,125,0,</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="E39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>0</v>
@@ -3337,15 +3745,15 @@
       <c r="P39" s="1"/>
       <c r="R39">
         <f t="shared" si="9"/>
-        <v>245</v>
+        <v>125</v>
       </c>
       <c r="S39">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>244</v>
       </c>
       <c r="T39">
         <f t="shared" si="11"/>
-        <v>253</v>
+        <v>125</v>
       </c>
       <c r="U39">
         <f t="shared" si="12"/>
@@ -3353,55 +3761,49 @@
       </c>
       <c r="W39" t="str">
         <f t="shared" si="4"/>
-        <v>245,1,253,0,</v>
+        <v>125,244,125,0,</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="I40" s="1"/>
       <c r="J40" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="R40">
         <f t="shared" si="9"/>
-        <v>255</v>
+        <v>20</v>
       </c>
       <c r="S40">
         <f t="shared" si="10"/>
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="T40">
         <f t="shared" si="11"/>
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="U40">
         <f t="shared" si="12"/>
@@ -3409,25 +3811,15 @@
       </c>
       <c r="W40" t="str">
         <f t="shared" si="4"/>
-        <v>255,64,85,0,</v>
+        <v>20,80,20,0,</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -3441,11 +3833,11 @@
       <c r="P41" s="1"/>
       <c r="R41">
         <f t="shared" si="9"/>
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="S41">
         <f t="shared" si="10"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="T41">
         <f t="shared" si="11"/>
@@ -3457,20 +3849,14 @@
       </c>
       <c r="W41" t="str">
         <f t="shared" si="4"/>
-        <v>127,64,0,0,</v>
+        <v>0,0,0,0,</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -3485,7 +3871,7 @@
       <c r="P42" s="1"/>
       <c r="R42">
         <f t="shared" si="9"/>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="S42">
         <f t="shared" si="10"/>
@@ -3501,7 +3887,7 @@
       </c>
       <c r="W42" t="str">
         <f t="shared" si="4"/>
-        <v>21,0,0,0,</v>
+        <v>0,0,0,0,</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Code cleanup Compass widget Vario graph widget Speedup OSD256_block_fill
</commit_message>
<xml_diff>
--- a/tools/16x20char_designer.xlsx
+++ b/tools/16x20char_designer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\00GIT\OSDeluxe\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68E07A0-EB59-4558-8A20-27DF42FD1B8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEA4A09-A963-4DC8-B746-D13C691CA7B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="9120" xr2:uid="{7204D92D-006B-4887-9E42-7235DD687936}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="3">
   <si>
     <t>x</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>o</t>
-  </si>
-  <si>
-    <t>oo</t>
   </si>
 </sst>
 </file>
@@ -421,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E001EF35-DD21-4C5D-9503-E7A7D79A3371}">
   <dimension ref="A1:BD44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25:W44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="W44" sqref="W25:W44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,84 +487,110 @@
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="R2">
         <f>IF(A2="o",64,0)+IF(A2="x",192,0)+IF(B2="o",16,0)+IF(B2="x",48,0)+IF(C2="o",4,0)+IF(C2="x",12,0)+IF(D2="o",1,0)+IF(D2="x",3,0)</f>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="S2">
         <f>IF(E2="o",64,0)+IF(E2="x",192,0)+IF(F2="o",16,0)+IF(F2="x",48,0)+IF(G2="o",4,0)+IF(G2="x",12,0)+IF(H2="o",1,0)+IF(H2="x",3,0)</f>
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="T2">
         <f>IF(I2="o",64,0)+IF(I2="x",192,0)+IF(J2="o",16,0)+IF(J2="x",48,0)+IF(K2="o",4,0)+IF(K2="x",12,0)+IF(L2="o",1,0)+IF(L2="x",3,0)</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="U2">
         <f>IF(M2="o",64,0)+IF(M2="x",192,0)+IF(N2="o",16,0)+IF(N2="x",48,0)+IF(O2="o",4,0)+IF(O2="x",12,0)+IF(P2="o",1,0)+IF(P2="x",3,0)</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="W2" t="str">
         <f>_xlfn.CONCAT(R2,",",S2,",",T2,",",U2,",")</f>
-        <v>20,5,0,0,</v>
+        <v>5,85,80,80,</v>
       </c>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
+      <c r="AB2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AE2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
+      <c r="AG2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
+      <c r="AJ2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="1"/>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
-      <c r="AR2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
@@ -580,21 +603,21 @@
       <c r="BD2" s="1"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>0</v>
@@ -603,53 +626,65 @@
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" t="s">
         <v>1</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R20" si="0">IF(A3="o",64,0)+IF(A3="x",192,0)+IF(B3="o",16,0)+IF(B3="x",48,0)+IF(C3="o",4,0)+IF(C3="x",12,0)+IF(D3="o",1,0)+IF(D3="x",3,0)</f>
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S20" si="1">IF(E3="o",64,0)+IF(E3="x",192,0)+IF(F3="o",16,0)+IF(F3="x",48,0)+IF(G3="o",4,0)+IF(G3="x",12,0)+IF(H3="o",1,0)+IF(H3="x",3,0)</f>
-        <v>31</v>
+        <v>255</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T20" si="2">IF(I3="o",64,0)+IF(I3="x",192,0)+IF(J3="o",16,0)+IF(J3="x",48,0)+IF(K3="o",4,0)+IF(K3="x",12,0)+IF(L3="o",1,0)+IF(L3="x",3,0)</f>
-        <v>64</v>
+        <v>245</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U20" si="3">IF(M3="o",64,0)+IF(M3="x",192,0)+IF(N3="o",16,0)+IF(N3="x",48,0)+IF(O3="o",4,0)+IF(O3="x",12,0)+IF(P3="o",1,0)+IF(P3="x",3,0)</f>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="W3" t="str">
         <f t="shared" ref="W3:W44" si="4">_xlfn.CONCAT(R3,",",S3,",",T3,",",U3,",")</f>
-        <v>125,31,64,0,</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>31,255,245,244,</v>
+      </c>
+      <c r="Y3" s="2"/>
       <c r="Z3" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC3" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AD3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE3" s="2" t="s">
         <v>0</v>
@@ -658,30 +693,34 @@
         <v>0</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AN3" s="2"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
-      <c r="AR3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
@@ -693,21 +732,21 @@
       <c r="BD3" s="1"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>0</v>
@@ -716,53 +755,65 @@
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="P4" s="2"/>
       <c r="Q4" t="s">
         <v>1</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>255</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>245</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="W4" t="str">
         <f t="shared" si="4"/>
-        <v>125,31,64,0,</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>31,255,245,244,</v>
+      </c>
+      <c r="Y4" s="2"/>
       <c r="Z4" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC4" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="AD4" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="2" t="s">
         <v>0</v>
@@ -771,30 +822,34 @@
         <v>0</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AN4" s="2"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
-      <c r="AR4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
@@ -806,131 +861,135 @@
       <c r="BD4" s="1"/>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s">
         <v>1</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="S5">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="4"/>
-        <v>125,31,64,0,</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>5,125,81,244,</v>
+      </c>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
       <c r="AA5" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AC5" s="2"/>
+      <c r="AC5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AD5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AH5" s="2"/>
+      <c r="AH5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AI5" s="2"/>
-      <c r="AJ5" s="2"/>
-      <c r="AK5" s="2"/>
-      <c r="AL5" s="2"/>
-      <c r="AM5" s="2"/>
+      <c r="AJ5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AN5" s="2"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
-      <c r="AR5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU5" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
       <c r="AX5" s="1"/>
       <c r="AY5" s="1"/>
       <c r="AZ5" s="1"/>
       <c r="BA5" s="1"/>
-      <c r="BB5" s="1"/>
-      <c r="BC5" s="1"/>
+      <c r="BB5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC5" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BD5" s="1"/>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
@@ -946,19 +1005,25 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="L6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="2"/>
       <c r="Q6" t="s">
         <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
@@ -966,28 +1031,20 @@
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="4"/>
-        <v>125,125,0,0,</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>0,125,1,244,</v>
+      </c>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
       <c r="AC6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1003,51 +1060,49 @@
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
-      <c r="AL6" s="2"/>
-      <c r="AM6" s="2"/>
-      <c r="AN6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN6" s="2"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
-      <c r="AR6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
       <c r="AY6" s="1"/>
       <c r="AZ6" s="1"/>
-      <c r="BA6" s="1"/>
-      <c r="BB6" s="1"/>
-      <c r="BC6" s="1"/>
-      <c r="BD6" s="1"/>
+      <c r="BA6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1067,16 +1122,20 @@
         <v>2</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="P7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
@@ -1088,24 +1147,16 @@
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>245</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="4"/>
-        <v>125,125,1,65,</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>0,125,1,245,</v>
+      </c>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
       <c r="AC7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1125,27 +1176,27 @@
         <v>2</v>
       </c>
       <c r="AK7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL7" s="2"/>
-      <c r="AM7" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AN7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AO7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AP7" s="1"/>
+      <c r="AP7" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AQ7" s="1"/>
-      <c r="AR7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
       <c r="AU7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1160,24 +1211,24 @@
       </c>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
-      <c r="BA7" s="1"/>
-      <c r="BB7" s="1"/>
-      <c r="BC7" s="1"/>
-      <c r="BD7" s="1"/>
+      <c r="BA7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1185,61 +1236,53 @@
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>215</v>
+        <v>255</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="4"/>
-        <v>125,116,7,215,</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>0,125,1,255,</v>
+      </c>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
       <c r="AC8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1247,25 +1290,25 @@
         <v>0</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF8" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
-      <c r="AI8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AI8" s="2"/>
       <c r="AJ8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN8" s="2" t="s">
         <v>0</v>
@@ -1274,17 +1317,15 @@
         <v>0</v>
       </c>
       <c r="AP8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ8" s="1"/>
-      <c r="AR8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS8" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
       <c r="AT8" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU8" s="1" t="s">
         <v>0</v>
@@ -1303,111 +1344,99 @@
       </c>
       <c r="AZ8" s="1"/>
       <c r="BA8" s="1"/>
-      <c r="BB8" s="1"/>
-      <c r="BC8" s="1"/>
+      <c r="BB8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC8" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BD8" s="1"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>125</v>
       </c>
       <c r="T9">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>215</v>
+        <v>255</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="4"/>
-        <v>127,208,31,215,</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>0,125,1,255,</v>
+      </c>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
       <c r="AC9" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE9" s="2"/>
-      <c r="AF9" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AG9" s="2"/>
-      <c r="AH9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI9" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
       <c r="AJ9" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM9" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN9" s="2" t="s">
         <v>0</v>
@@ -1419,13 +1448,13 @@
         <v>0</v>
       </c>
       <c r="AQ9" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="AS9" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT9" s="1" t="s">
         <v>0</v>
@@ -1454,114 +1483,90 @@
       <c r="BD9" s="1"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="R10">
         <f t="shared" si="0"/>
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>245</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="4"/>
-        <v>127,244,125,125,</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>0,125,1,245,</v>
+      </c>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
       <c r="AC10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
       <c r="AJ10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AM10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN10" s="2" t="s">
         <v>2</v>
@@ -1579,13 +1584,13 @@
         <v>2</v>
       </c>
       <c r="AS10" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AV10" s="1" t="s">
         <v>2</v>
@@ -1608,18 +1613,10 @@
       <c r="BD10" s="1"/>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1632,33 +1629,25 @@
       <c r="H11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="P11" s="2"/>
       <c r="R11">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
@@ -1666,28 +1655,20 @@
       </c>
       <c r="T11">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="U11">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="4"/>
-        <v>125,125,125,125,</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>0,125,1,244,</v>
+      </c>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
       <c r="AC11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1700,30 +1681,22 @@
       <c r="AF11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AG11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI11" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
       <c r="AJ11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AM11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN11" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AN11" s="2"/>
       <c r="AO11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1737,45 +1710,35 @@
         <v>2</v>
       </c>
       <c r="AS11" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AU11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV11" s="1"/>
-      <c r="AW11" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AV11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW11" s="1"/>
       <c r="AX11" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ11" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AZ11" s="1"/>
       <c r="BA11" s="1"/>
       <c r="BB11" s="1"/>
       <c r="BC11" s="1"/>
       <c r="BD11" s="1"/>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
@@ -1788,33 +1751,25 @@
       <c r="H12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="P12" s="2"/>
       <c r="R12">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
@@ -1822,28 +1777,20 @@
       </c>
       <c r="T12">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="U12">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="4"/>
-        <v>125,125,125,125,</v>
-      </c>
-      <c r="Y12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>0,125,1,244,</v>
+      </c>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
       <c r="AC12" s="2" t="s">
         <v>2</v>
       </c>
@@ -1856,30 +1803,22 @@
       <c r="AF12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AG12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI12" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
       <c r="AJ12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK12" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AM12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN12" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AN12" s="2"/>
       <c r="AO12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1893,145 +1832,111 @@
         <v>2</v>
       </c>
       <c r="AS12" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AU12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV12" s="1"/>
-      <c r="AW12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ12" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AV12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
       <c r="BA12" s="1"/>
       <c r="BB12" s="1"/>
       <c r="BC12" s="1"/>
       <c r="BD12" s="1"/>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="P13" s="2"/>
       <c r="R13">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="T13">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="U13">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="4"/>
-        <v>125,31,125,125,</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC13" s="2"/>
+        <v>0,125,1,244,</v>
+      </c>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AD13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
       <c r="AJ13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK13" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AM13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AN13" s="2"/>
       <c r="AO13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2045,145 +1950,115 @@
         <v>2</v>
       </c>
       <c r="AS13" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AU13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV13" s="1"/>
-      <c r="AW13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ13" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AV13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
       <c r="BA13" s="1"/>
-      <c r="BB13" s="1"/>
-      <c r="BC13" s="1"/>
+      <c r="BB13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC13" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BD13" s="1"/>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="P14" s="2"/>
       <c r="R14">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="U14">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="W14" t="str">
         <f t="shared" si="4"/>
-        <v>125,31,125,125,</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC14" s="2"/>
+        <v>0,125,1,244,</v>
+      </c>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AD14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
       <c r="AJ14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK14" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AM14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN14" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AN14" s="2"/>
       <c r="AO14" s="1" t="s">
         <v>2</v>
       </c>
@@ -2197,145 +2072,119 @@
         <v>2</v>
       </c>
       <c r="AS14" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AU14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV14" s="1"/>
-      <c r="AW14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA14" s="1"/>
-      <c r="BB14" s="1"/>
-      <c r="BC14" s="1"/>
-      <c r="BD14" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AV14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+      <c r="BA14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD14" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="2"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="P15" s="2"/>
       <c r="R15">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="T15">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="U15">
         <f t="shared" si="3"/>
-        <v>61</v>
+        <v>244</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="4"/>
-        <v>125,31,125,61,</v>
-      </c>
-      <c r="Y15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC15" s="2"/>
+        <v>0,125,1,244,</v>
+      </c>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AD15" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
       <c r="AJ15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK15" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AL15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AM15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN15" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AN15" s="2"/>
       <c r="AO15" s="1" t="s">
         <v>2</v>
       </c>
@@ -2349,145 +2198,119 @@
         <v>2</v>
       </c>
       <c r="AS15" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AU15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV15" s="1"/>
-      <c r="AW15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BA15" s="1"/>
-      <c r="BB15" s="1"/>
-      <c r="BC15" s="1"/>
-      <c r="BD15" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AV15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD15" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="2"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="P16" s="2"/>
       <c r="R16">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="S16">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="T16">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="U16">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="4"/>
-        <v>125,31,125,125,</v>
-      </c>
-      <c r="Y16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC16" s="2"/>
+        <v>0,125,1,244,</v>
+      </c>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AD16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AF16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
       <c r="AJ16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK16" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AM16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN16" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AN16" s="2"/>
       <c r="AO16" s="1" t="s">
         <v>2</v>
       </c>
@@ -2501,120 +2324,98 @@
         <v>2</v>
       </c>
       <c r="AS16" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AU16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV16" s="1"/>
-      <c r="AW16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ16" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AV16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
       <c r="BA16" s="1"/>
-      <c r="BB16" s="1"/>
-      <c r="BC16" s="1"/>
+      <c r="BB16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC16" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BD16" s="1"/>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="G17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="N17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="R17">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T17">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="U17">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="4"/>
-        <v>20,5,20,20,</v>
+        <v>0,20,0,80,</v>
       </c>
       <c r="Y17" s="2"/>
-      <c r="Z17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
+      <c r="AD17" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AE17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AF17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
-      <c r="AH17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AL17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AM17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="1"/>
       <c r="AP17" s="1" t="s">
@@ -2624,21 +2425,17 @@
         <v>2</v>
       </c>
       <c r="AR17" s="1"/>
-      <c r="AS17" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AS17" s="1"/>
       <c r="AT17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AU17" s="1"/>
+      <c r="AU17" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
-      <c r="AX17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY17" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
       <c r="AZ17" s="1"/>
       <c r="BA17" s="1"/>
       <c r="BB17" s="1"/>
@@ -2944,15 +2741,9 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2969,7 +2760,7 @@
       </c>
       <c r="S25">
         <f>IF(E25="o",64,0)+IF(E25="x",192,0)+IF(F25="o",16,0)+IF(F25="x",48,0)+IF(G25="o",4,0)+IF(G25="x",12,0)+IF(H25="o",1,0)+IF(H25="x",3,0)</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="T25">
         <f>IF(I25="o",64,0)+IF(I25="x",192,0)+IF(J25="o",16,0)+IF(J25="x",48,0)+IF(K25="o",4,0)+IF(K25="x",12,0)+IF(L25="o",1,0)+IF(L25="x",3,0)</f>
@@ -2981,25 +2772,17 @@
       </c>
       <c r="W25" t="str">
         <f t="shared" si="4"/>
-        <v>0,80,0,0,</v>
+        <v>0,0,0,0,</v>
       </c>
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -3011,11 +2794,11 @@
       <c r="P26" s="1"/>
       <c r="R26">
         <f t="shared" ref="R26:R44" si="9">IF(A26="o",64,0)+IF(A26="x",192,0)+IF(B26="o",16,0)+IF(B26="x",48,0)+IF(C26="o",4,0)+IF(C26="x",12,0)+IF(D26="o",1,0)+IF(D26="x",3,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26">
         <f t="shared" ref="S26:S44" si="10">IF(E26="o",64,0)+IF(E26="x",192,0)+IF(F26="o",16,0)+IF(F26="x",48,0)+IF(G26="o",4,0)+IF(G26="x",12,0)+IF(H26="o",1,0)+IF(H26="x",3,0)</f>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="T26">
         <f t="shared" ref="T26:T44" si="11">IF(I26="o",64,0)+IF(I26="x",192,0)+IF(J26="o",16,0)+IF(J26="x",48,0)+IF(K26="o",4,0)+IF(K26="x",12,0)+IF(L26="o",1,0)+IF(L26="x",3,0)</f>
@@ -3027,25 +2810,17 @@
       </c>
       <c r="W26" t="str">
         <f t="shared" si="4"/>
-        <v>1,244,0,0,</v>
+        <v>0,0,0,0,</v>
       </c>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -3057,11 +2832,11 @@
       <c r="P27" s="1"/>
       <c r="R27">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="T27">
         <f t="shared" si="11"/>
@@ -3073,41 +2848,37 @@
       </c>
       <c r="W27" t="str">
         <f t="shared" si="4"/>
-        <v>1,244,0,0,</v>
+        <v>0,0,0,0,</v>
       </c>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
+      <c r="N28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="P28" s="1"/>
       <c r="R28">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S28">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="T28">
         <f t="shared" si="11"/>
@@ -3115,45 +2886,45 @@
       </c>
       <c r="U28">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W28" t="str">
         <f t="shared" si="4"/>
-        <v>1,244,0,0,</v>
+        <v>0,0,0,20,</v>
       </c>
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="R29">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S29">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="T29">
         <f t="shared" si="11"/>
@@ -3161,28 +2932,24 @@
       </c>
       <c r="U29">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="W29" t="str">
         <f t="shared" si="4"/>
-        <v>1,244,0,0,</v>
+        <v>0,0,0,125,</v>
       </c>
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
         <v>2</v>
       </c>
@@ -3197,17 +2964,25 @@
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
+      <c r="M30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="R30">
         <f t="shared" si="9"/>
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="S30">
         <f t="shared" si="10"/>
-        <v>245</v>
+        <v>5</v>
       </c>
       <c r="T30">
         <f t="shared" si="11"/>
@@ -3215,11 +2990,11 @@
       </c>
       <c r="U30">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="W30" t="str">
         <f t="shared" si="4"/>
-        <v>65,245,80,0,</v>
+        <v>80,5,80,125,</v>
       </c>
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.25">
@@ -3227,17 +3002,15 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>0</v>
@@ -3256,16 +3029,20 @@
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
+      <c r="N31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="P31" s="1"/>
       <c r="R31">
         <f t="shared" si="9"/>
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="S31">
         <f t="shared" si="10"/>
-        <v>255</v>
+        <v>31</v>
       </c>
       <c r="T31">
         <f t="shared" si="11"/>
@@ -3273,11 +3050,11 @@
       </c>
       <c r="U31">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W31" t="str">
         <f t="shared" si="4"/>
-        <v>209,255,244,0,</v>
+        <v>244,31,244,20,</v>
       </c>
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.25">
@@ -3288,13 +3065,13 @@
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>0</v>
@@ -3323,11 +3100,11 @@
       <c r="P32" s="1"/>
       <c r="R32">
         <f t="shared" si="9"/>
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="S32">
         <f t="shared" si="10"/>
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="T32">
         <f t="shared" si="11"/>
@@ -3339,7 +3116,7 @@
       </c>
       <c r="W32" t="str">
         <f t="shared" si="4"/>
-        <v>245,255,253,0,</v>
+        <v>253,127,253,0,</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -3356,13 +3133,13 @@
         <v>2</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>2</v>
@@ -3389,7 +3166,7 @@
       </c>
       <c r="S33">
         <f t="shared" si="10"/>
-        <v>245</v>
+        <v>125</v>
       </c>
       <c r="T33">
         <f t="shared" si="11"/>
@@ -3401,7 +3178,7 @@
       </c>
       <c r="W33" t="str">
         <f t="shared" si="4"/>
-        <v>125,245,125,0,</v>
+        <v>125,125,125,0,</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -3418,27 +3195,25 @@
         <v>2</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I34" s="1"/>
       <c r="J34" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -3449,11 +3224,11 @@
       </c>
       <c r="S34">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="T34">
         <f t="shared" si="11"/>
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="U34">
         <f t="shared" si="12"/>
@@ -3461,7 +3236,7 @@
       </c>
       <c r="W34" t="str">
         <f t="shared" si="4"/>
-        <v>125,244,125,0,</v>
+        <v>125,125,20,0,</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
@@ -3478,27 +3253,21 @@
         <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -3509,11 +3278,11 @@
       </c>
       <c r="S35">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="T35">
         <f t="shared" si="11"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="U35">
         <f t="shared" si="12"/>
@@ -3521,7 +3290,7 @@
       </c>
       <c r="W35" t="str">
         <f t="shared" si="4"/>
-        <v>125,244,125,0,</v>
+        <v>125,125,0,0,</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
@@ -3538,30 +3307,28 @@
         <v>2</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
+      <c r="N36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="P36" s="1"/>
       <c r="R36">
         <f t="shared" si="9"/>
@@ -3569,19 +3336,19 @@
       </c>
       <c r="S36">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="T36">
         <f t="shared" si="11"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="U36">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W36" t="str">
         <f t="shared" si="4"/>
-        <v>125,244,125,0,</v>
+        <v>125,125,0,20,</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -3598,50 +3365,52 @@
         <v>2</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="R37">
         <f t="shared" si="9"/>
         <v>125</v>
       </c>
       <c r="S37">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="T37">
         <f t="shared" si="11"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="U37">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="W37" t="str">
         <f t="shared" si="4"/>
-        <v>125,244,125,0,</v>
+        <v>125,125,0,125,</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -3658,50 +3427,52 @@
         <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="R38">
         <f t="shared" si="9"/>
         <v>125</v>
       </c>
       <c r="S38">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="T38">
         <f t="shared" si="11"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="U38">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="W38" t="str">
         <f t="shared" si="4"/>
-        <v>125,244,125,0,</v>
+        <v>125,125,0,125,</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -3718,30 +3489,28 @@
         <v>2</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
+      <c r="N39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="P39" s="1"/>
       <c r="R39">
         <f t="shared" si="9"/>
@@ -3749,19 +3518,19 @@
       </c>
       <c r="S39">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="T39">
         <f t="shared" si="11"/>
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="U39">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W39" t="str">
         <f t="shared" si="4"/>
-        <v>125,244,125,0,</v>
+        <v>125,125,0,20,</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
@@ -3773,21 +3542,17 @@
         <v>2</v>
       </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="1"/>
+      <c r="G40" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
@@ -3799,11 +3564,11 @@
       </c>
       <c r="S40">
         <f t="shared" si="10"/>
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="T40">
         <f t="shared" si="11"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="U40">
         <f t="shared" si="12"/>
@@ -3811,7 +3576,7 @@
       </c>
       <c r="W40" t="str">
         <f t="shared" si="4"/>
-        <v>20,80,20,0,</v>
+        <v>20,20,0,0,</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add rssi moved string to strings.h Do some code cleanup for clean compile
</commit_message>
<xml_diff>
--- a/tools/16x20char_designer.xlsx
+++ b/tools/16x20char_designer.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\00GIT\OSDeluxe\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEA4A09-A963-4DC8-B746-D13C691CA7B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D512239D-6778-4F73-B222-F6343250C2EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="9120" xr2:uid="{7204D92D-006B-4887-9E42-7235DD687936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="3">
   <si>
     <t>x</t>
   </si>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E001EF35-DD21-4C5D-9503-E7A7D79A3371}">
   <dimension ref="A1:BD44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="W44" sqref="W25:W44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,102 +487,66 @@
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="2"/>
+      <c r="O2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="P2" s="2"/>
       <c r="R2">
         <f>IF(A2="o",64,0)+IF(A2="x",192,0)+IF(B2="o",16,0)+IF(B2="x",48,0)+IF(C2="o",4,0)+IF(C2="x",12,0)+IF(D2="o",1,0)+IF(D2="x",3,0)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S2">
         <f>IF(E2="o",64,0)+IF(E2="x",192,0)+IF(F2="o",16,0)+IF(F2="x",48,0)+IF(G2="o",4,0)+IF(G2="x",12,0)+IF(H2="o",1,0)+IF(H2="x",3,0)</f>
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="T2">
         <f>IF(I2="o",64,0)+IF(I2="x",192,0)+IF(J2="o",16,0)+IF(J2="x",48,0)+IF(K2="o",4,0)+IF(K2="x",12,0)+IF(L2="o",1,0)+IF(L2="x",3,0)</f>
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="U2">
         <f>IF(M2="o",64,0)+IF(M2="x",192,0)+IF(N2="o",16,0)+IF(N2="x",48,0)+IF(O2="o",4,0)+IF(O2="x",12,0)+IF(P2="o",1,0)+IF(P2="x",3,0)</f>
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="W2" t="str">
         <f>_xlfn.CONCAT(R2,",",S2,",",T2,",",U2,",")</f>
-        <v>5,85,80,80,</v>
+        <v>20,1,64,20,</v>
       </c>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
-      <c r="AJ2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="1"/>
@@ -603,24 +567,22 @@
       <c r="BD2" s="1"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>0</v>
@@ -629,90 +591,60 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="Q3" t="s">
         <v>1</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R20" si="0">IF(A3="o",64,0)+IF(A3="x",192,0)+IF(B3="o",16,0)+IF(B3="x",48,0)+IF(C3="o",4,0)+IF(C3="x",12,0)+IF(D3="o",1,0)+IF(D3="x",3,0)</f>
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S20" si="1">IF(E3="o",64,0)+IF(E3="x",192,0)+IF(F3="o",16,0)+IF(F3="x",48,0)+IF(G3="o",4,0)+IF(G3="x",12,0)+IF(H3="o",1,0)+IF(H3="x",3,0)</f>
-        <v>255</v>
+        <v>7</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T20" si="2">IF(I3="o",64,0)+IF(I3="x",192,0)+IF(J3="o",16,0)+IF(J3="x",48,0)+IF(K3="o",4,0)+IF(K3="x",12,0)+IF(L3="o",1,0)+IF(L3="x",3,0)</f>
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U20" si="3">IF(M3="o",64,0)+IF(M3="x",192,0)+IF(N3="o",16,0)+IF(N3="x",48,0)+IF(O3="o",4,0)+IF(O3="x",12,0)+IF(P3="o",1,0)+IF(P3="x",3,0)</f>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="W3" t="str">
         <f t="shared" ref="W3:W44" si="4">_xlfn.CONCAT(R3,",",S3,",",T3,",",U3,",")</f>
-        <v>31,255,245,244,</v>
+        <v>125,7,208,125,</v>
       </c>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
@@ -732,24 +664,22 @@
       <c r="BD3" s="1"/>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
@@ -758,90 +688,60 @@
         <v>0</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="Q4" t="s">
         <v>1</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>7</v>
       </c>
       <c r="T4">
         <f t="shared" si="2"/>
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="W4" t="str">
         <f t="shared" si="4"/>
-        <v>31,255,245,244,</v>
+        <v>125,7,208,125,</v>
       </c>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
@@ -862,27 +762,27 @@
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>2</v>
@@ -906,15 +806,15 @@
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="S5">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>81</v>
+        <v>209</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
@@ -922,47 +822,23 @@
       </c>
       <c r="W5" t="str">
         <f t="shared" si="4"/>
-        <v>5,125,81,244,</v>
+        <v>31,71,209,244,</v>
       </c>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
-      <c r="AA5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
-      <c r="AJ5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
@@ -977,33 +853,37 @@
       <c r="AY5" s="1"/>
       <c r="AZ5" s="1"/>
       <c r="BA5" s="1"/>
-      <c r="BB5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC5" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
       <c r="BD5" s="1"/>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
         <v>2</v>
@@ -1023,15 +903,15 @@
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>209</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
@@ -1039,39 +919,23 @@
       </c>
       <c r="W6" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,244,</v>
+        <v>31,71,209,244,</v>
       </c>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-      <c r="AC6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
-      <c r="AJ6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
@@ -1085,398 +949,284 @@
       <c r="AX6" s="1"/>
       <c r="AY6" s="1"/>
       <c r="AZ6" s="1"/>
-      <c r="BA6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BC6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BD6" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E7" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="L7" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="T7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>215</v>
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,245,</v>
+        <v>7,215,215,208,</v>
       </c>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
-      <c r="AC7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
-      <c r="AJ7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP7" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
       <c r="AR7" s="1"/>
       <c r="AS7" s="1"/>
       <c r="AT7" s="1"/>
-      <c r="AU7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX7" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
-      <c r="BA7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BD7" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="1"/>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="L8" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S8">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="T8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>215</v>
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>255</v>
+        <v>208</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,255,</v>
+        <v>7,215,215,208,</v>
       </c>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
-      <c r="AC8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
-      <c r="AJ8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
       <c r="AR8" s="1"/>
       <c r="AS8" s="1"/>
-      <c r="AT8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AW8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY8" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="1"/>
       <c r="AZ8" s="1"/>
       <c r="BA8" s="1"/>
-      <c r="BB8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC8" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
       <c r="BD8" s="1"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E9" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="L9" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>247</v>
       </c>
       <c r="T9">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>223</v>
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>255</v>
+        <v>64</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,255,</v>
+        <v>1,247,223,64,</v>
       </c>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-      <c r="AC9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
-      <c r="AJ9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ9" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
       <c r="BA9" s="1"/>
       <c r="BB9" s="1"/>
       <c r="BC9" s="1"/>
@@ -1486,127 +1236,87 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="L10" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
       <c r="R10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>247</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>223</v>
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>245</v>
+        <v>64</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,245,</v>
+        <v>1,247,223,64,</v>
       </c>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
-      <c r="AC10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
-      <c r="AJ10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AY10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ10" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
       <c r="BA10" s="1"/>
       <c r="BB10" s="1"/>
       <c r="BC10" s="1"/>
@@ -1627,23 +1337,23 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="L11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="R11">
         <f t="shared" si="0"/>
@@ -1651,83 +1361,47 @@
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="T11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>253</v>
       </c>
       <c r="U11">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,244,</v>
+        <v>0,127,253,0,</v>
       </c>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
-      <c r="AC11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
-      <c r="AJ11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM11" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
-      <c r="AO11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV11" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
       <c r="AW11" s="1"/>
-      <c r="AX11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY11" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
       <c r="AZ11" s="1"/>
       <c r="BA11" s="1"/>
       <c r="BB11" s="1"/>
@@ -1749,23 +1423,23 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="L12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="R12">
         <f t="shared" si="0"/>
@@ -1773,76 +1447,44 @@
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="T12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>253</v>
       </c>
       <c r="U12">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,244,</v>
+        <v>0,127,253,0,</v>
       </c>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
-      <c r="AC12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
-      <c r="AJ12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM12" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
-      <c r="AO12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV12" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
       <c r="AW12" s="1"/>
       <c r="AX12" s="1"/>
       <c r="AY12" s="1"/>
@@ -1857,33 +1499,31 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="L13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="R13">
         <f t="shared" si="0"/>
@@ -1891,87 +1531,51 @@
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="T13">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>244</v>
       </c>
       <c r="U13">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,244,</v>
+        <v>0,31,244,0,</v>
       </c>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
-      <c r="AC13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
-      <c r="AJ13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
-      <c r="AO13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV13" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
       <c r="AW13" s="1"/>
       <c r="AX13" s="1"/>
       <c r="AY13" s="1"/>
       <c r="AZ13" s="1"/>
       <c r="BA13" s="1"/>
-      <c r="BB13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC13" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="BB13" s="1"/>
+      <c r="BC13" s="1"/>
       <c r="BD13" s="1"/>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
@@ -1979,33 +1583,25 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="R14">
         <f t="shared" si="0"/>
@@ -2013,125 +1609,77 @@
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>208</v>
       </c>
       <c r="U14">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="W14" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,244,</v>
+        <v>0,7,208,0,</v>
       </c>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
-      <c r="AC14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
-      <c r="AJ14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM14" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
-      <c r="AO14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV14" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
       <c r="AX14" s="1"/>
       <c r="AY14" s="1"/>
       <c r="AZ14" s="1"/>
-      <c r="BA14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BC14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BD14" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="BA14" s="1"/>
+      <c r="BB14" s="1"/>
+      <c r="BC14" s="1"/>
+      <c r="BD14" s="1"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="R15">
         <f t="shared" si="0"/>
@@ -2139,125 +1687,77 @@
       </c>
       <c r="S15">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="T15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>208</v>
       </c>
       <c r="U15">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,244,</v>
+        <v>0,7,208,0,</v>
       </c>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
-      <c r="AC15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
-      <c r="AJ15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM15" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
-      <c r="AO15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV15" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
       <c r="AW15" s="1"/>
       <c r="AX15" s="1"/>
       <c r="AY15" s="1"/>
       <c r="AZ15" s="1"/>
-      <c r="BA15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BC15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BD15" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="1"/>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="R16">
         <f t="shared" si="0"/>
@@ -2265,87 +1765,51 @@
       </c>
       <c r="S16">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="T16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>208</v>
       </c>
       <c r="U16">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>0</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="4"/>
-        <v>0,125,1,244,</v>
+        <v>0,7,208,0,</v>
       </c>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
-      <c r="AC16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
-      <c r="AJ16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM16" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
-      <c r="AO16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV16" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
       <c r="AW16" s="1"/>
       <c r="AX16" s="1"/>
       <c r="AY16" s="1"/>
       <c r="AZ16" s="1"/>
       <c r="BA16" s="1"/>
-      <c r="BB16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="BC16" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="BB16" s="1"/>
+      <c r="BC16" s="1"/>
       <c r="BD16" s="1"/>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.25">
@@ -2354,23 +1818,23 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="R17">
@@ -2379,59 +1843,43 @@
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="T17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="U17">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="4"/>
-        <v>0,20,0,80,</v>
+        <v>0,7,208,0,</v>
       </c>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
-      <c r="AK17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL17" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="1"/>
-      <c r="AP17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ17" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
       <c r="AR17" s="1"/>
       <c r="AS17" s="1"/>
-      <c r="AT17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU17" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
       <c r="AX17" s="1"/>
@@ -2449,10 +1897,18 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -2465,11 +1921,11 @@
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="U18">
         <f t="shared" si="3"/>
@@ -2477,7 +1933,7 @@
       </c>
       <c r="W18" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,</v>
+        <v>0,7,208,0,</v>
       </c>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
@@ -2519,10 +1975,18 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -2535,11 +1999,11 @@
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="U19">
         <f t="shared" si="3"/>
@@ -2547,7 +2011,7 @@
       </c>
       <c r="W19" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,</v>
+        <v>0,7,208,0,</v>
       </c>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
@@ -2589,10 +2053,18 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -2605,11 +2077,11 @@
       </c>
       <c r="S20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="U20">
         <f t="shared" si="3"/>
@@ -2617,7 +2089,7 @@
       </c>
       <c r="W20" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,</v>
+        <v>0,7,208,0,</v>
       </c>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
@@ -2660,8 +2132,12 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -2675,11 +2151,11 @@
       </c>
       <c r="S21">
         <f t="shared" ref="S21" si="6">IF(E21="o",64,0)+IF(E21="x",192,0)+IF(F21="o",16,0)+IF(F21="x",48,0)+IF(G21="o",4,0)+IF(G21="x",12,0)+IF(H21="o",1,0)+IF(H21="x",3,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21">
         <f t="shared" ref="T21" si="7">IF(I21="o",64,0)+IF(I21="x",192,0)+IF(J21="o",16,0)+IF(J21="x",48,0)+IF(K21="o",4,0)+IF(K21="x",12,0)+IF(L21="o",1,0)+IF(L21="x",3,0)</f>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="U21">
         <f t="shared" ref="U21" si="8">IF(M21="o",64,0)+IF(M21="x",192,0)+IF(N21="o",16,0)+IF(N21="x",48,0)+IF(O21="o",4,0)+IF(O21="x",12,0)+IF(P21="o",1,0)+IF(P21="x",3,0)</f>
@@ -2687,7 +2163,7 @@
       </c>
       <c r="W21" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,</v>
+        <v>0,1,64,0,</v>
       </c>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>

</xml_diff>